<commit_message>
adding missing eye scan registers, from the separate table in the middle of the document
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/xc7vx690tffg1927-2_GTH.xlsx
+++ b/examples/EMTF_MPCX_full/src/xc7vx690tffg1927-2_GTH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V7_GTH_atts_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5219" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5311" uniqueCount="1156">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -2888,6 +2888,63 @@
   </si>
   <si>
     <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Extra ES registers from Table 4-28: DRP Address Map for Eye Scan Read-Only (R) Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es_error_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es_sample_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es_control_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es_rdata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es_sdata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15D</t>
   </si>
   <si>
     <t xml:space="preserve">common_drp_map.tab</t>
@@ -13788,12 +13845,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G582"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A583" activeCellId="0" sqref="A583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22911,6 +22968,312 @@
         <v>947</v>
       </c>
     </row>
+    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A583" s="2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A584" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="B584" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C584" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D584" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="E584" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F584" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G584" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A585" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="B585" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C585" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D585" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="E585" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F585" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G585" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A586" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="B586" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="C586" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D586" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="E586" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F586" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G586" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A587" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="B587" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C587" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D587" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="E587" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F587" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G587" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A588" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="B588" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C588" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D588" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="E588" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F588" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G588" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A589" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="B589" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C589" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D589" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="E589" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="F589" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G589" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A590" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="B590" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C590" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D590" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="E590" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="F590" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G590" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A591" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="B591" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C591" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D591" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="E591" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F591" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G591" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A592" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="B592" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C592" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D592" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E592" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F592" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G592" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A593" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B593" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C593" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D593" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E593" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F593" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G593" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A594" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B594" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C594" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D594" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E594" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="F594" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G594" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A595" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="B595" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C595" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D595" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E595" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="F595" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G595" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A596" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="B596" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C596" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D596" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E596" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F596" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G596" s="5" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -22929,7 +23292,7 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
@@ -22964,7 +23327,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>952</v>
+        <v>971</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -23019,7 +23382,7 @@
         <v>646</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>953</v>
+        <v>972</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>743</v>
@@ -23036,13 +23399,13 @@
         <v>775</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>954</v>
+        <v>973</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>646</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>955</v>
+        <v>974</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>706</v>
@@ -23065,7 +23428,7 @@
         <v>646</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>953</v>
+        <v>972</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>837</v>
@@ -23088,7 +23451,7 @@
         <v>646</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>956</v>
+        <v>975</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>743</v>
@@ -23111,7 +23474,7 @@
         <v>646</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>957</v>
+        <v>976</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>660</v>
@@ -23214,10 +23577,10 @@
         <v>646</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>956</v>
+        <v>975</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>958</v>
+        <v>977</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>751</v>
@@ -23237,7 +23600,7 @@
         <v>646</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>959</v>
+        <v>978</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>743</v>
@@ -23260,7 +23623,7 @@
         <v>646</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>960</v>
+        <v>979</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>713</v>
@@ -23283,7 +23646,7 @@
         <v>646</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>961</v>
+        <v>980</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>792</v>
@@ -23306,7 +23669,7 @@
         <v>646</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>962</v>
+        <v>981</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>647</v>
@@ -23329,7 +23692,7 @@
         <v>646</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>963</v>
+        <v>982</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>647</v>
@@ -23352,7 +23715,7 @@
         <v>646</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>964</v>
+        <v>983</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>647</v>
@@ -23375,7 +23738,7 @@
         <v>646</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>965</v>
+        <v>984</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>647</v>
@@ -23398,7 +23761,7 @@
         <v>646</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>966</v>
+        <v>985</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>792</v>
@@ -23421,7 +23784,7 @@
         <v>646</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>967</v>
+        <v>986</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>647</v>
@@ -23438,13 +23801,13 @@
         <v>781</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>968</v>
+        <v>987</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>646</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>969</v>
+        <v>988</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>706</v>
@@ -23467,7 +23830,7 @@
         <v>646</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>970</v>
+        <v>989</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>743</v>
@@ -23490,7 +23853,7 @@
         <v>646</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>971</v>
+        <v>990</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>743</v>
@@ -23513,7 +23876,7 @@
         <v>646</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>971</v>
+        <v>990</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>768</v>
@@ -23536,7 +23899,7 @@
         <v>646</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>971</v>
+        <v>990</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>770</v>
@@ -23559,7 +23922,7 @@
         <v>646</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>971</v>
+        <v>990</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>772</v>
@@ -23573,7 +23936,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>972</v>
+        <v>991</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>743</v>
@@ -23582,7 +23945,7 @@
         <v>646</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>973</v>
+        <v>992</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>743</v>
@@ -23596,7 +23959,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>974</v>
+        <v>993</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>743</v>
@@ -23605,7 +23968,7 @@
         <v>646</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>975</v>
+        <v>994</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>743</v>
@@ -23628,7 +23991,7 @@
         <v>646</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>975</v>
+        <v>994</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>768</v>
@@ -23651,7 +24014,7 @@
         <v>646</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>976</v>
+        <v>995</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>702</v>
@@ -23674,7 +24037,7 @@
         <v>646</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>977</v>
+        <v>996</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>647</v>
@@ -23697,7 +24060,7 @@
         <v>646</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>978</v>
+        <v>997</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>702</v>
@@ -23757,7 +24120,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>979</v>
+        <v>998</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -23780,46 +24143,46 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>980</v>
+        <v>999</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>981</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>982</v>
+        <v>1001</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>983</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>984</v>
+        <v>1003</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>985</v>
+        <v>1004</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>986</v>
+        <v>1005</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>987</v>
+        <v>1006</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>988</v>
+        <v>1007</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>989</v>
+        <v>1008</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>990</v>
+        <v>1009</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>991</v>
+        <v>1010</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>992</v>
+        <v>1011</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>993</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23836,10 +24199,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>994</v>
+        <v>1013</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>995</v>
+        <v>1014</v>
       </c>
       <c r="I5" s="2" t="str">
         <f aca="false">E9</f>
@@ -23864,10 +24227,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>994</v>
+        <v>1013</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>995</v>
+        <v>1014</v>
       </c>
       <c r="I6" s="2" t="str">
         <f aca="false">E10</f>
@@ -23892,10 +24255,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>994</v>
+        <v>1013</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>995</v>
+        <v>1014</v>
       </c>
       <c r="I7" s="2" t="str">
         <f aca="false">E11</f>
@@ -23920,10 +24283,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>994</v>
+        <v>1013</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>995</v>
+        <v>1014</v>
       </c>
       <c r="I8" s="2" t="str">
         <f aca="false">E12</f>
@@ -23949,10 +24312,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>996</v>
+        <v>1015</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>997</v>
+        <v>1016</v>
       </c>
       <c r="G9" s="2" t="str">
         <f aca="false">E5</f>
@@ -23986,10 +24349,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>996</v>
+        <v>1015</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>997</v>
+        <v>1016</v>
       </c>
       <c r="G10" s="2" t="str">
         <f aca="false">E6</f>
@@ -24023,10 +24386,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>996</v>
+        <v>1015</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>997</v>
+        <v>1016</v>
       </c>
       <c r="G11" s="2" t="str">
         <f aca="false">E7</f>
@@ -24060,10 +24423,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>996</v>
+        <v>1015</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>997</v>
+        <v>1016</v>
       </c>
       <c r="G12" s="2" t="str">
         <f aca="false">E8</f>
@@ -24097,10 +24460,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>998</v>
+        <v>1017</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>999</v>
+        <v>1018</v>
       </c>
       <c r="G13" s="2" t="str">
         <f aca="false">E9</f>
@@ -24134,10 +24497,10 @@
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>998</v>
+        <v>1017</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>999</v>
+        <v>1018</v>
       </c>
       <c r="G14" s="2" t="str">
         <f aca="false">E10</f>
@@ -24171,10 +24534,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>998</v>
+        <v>1017</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>999</v>
+        <v>1018</v>
       </c>
       <c r="G15" s="2" t="str">
         <f aca="false">E11</f>
@@ -24208,10 +24571,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>998</v>
+        <v>1017</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>999</v>
+        <v>1018</v>
       </c>
       <c r="G16" s="2" t="str">
         <f aca="false">E12</f>
@@ -24245,10 +24608,10 @@
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1000</v>
+        <v>1019</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1001</v>
+        <v>1020</v>
       </c>
       <c r="G17" s="2" t="str">
         <f aca="false">E13</f>
@@ -24282,10 +24645,10 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1000</v>
+        <v>1019</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>1001</v>
+        <v>1020</v>
       </c>
       <c r="G18" s="2" t="str">
         <f aca="false">E14</f>
@@ -24319,10 +24682,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1000</v>
+        <v>1019</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>1001</v>
+        <v>1020</v>
       </c>
       <c r="G19" s="2" t="str">
         <f aca="false">E15</f>
@@ -24356,10 +24719,10 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>1000</v>
+        <v>1019</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>1001</v>
+        <v>1020</v>
       </c>
       <c r="G20" s="2" t="str">
         <f aca="false">E16</f>
@@ -26827,7 +27190,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1002</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26840,205 +27203,205 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1003</v>
+        <v>1022</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1004</v>
+        <v>1023</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1005</v>
+        <v>1024</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1006</v>
+        <v>1025</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>594</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1007</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1008</v>
+        <v>1027</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1010</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1008</v>
+        <v>1027</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1011</v>
+        <v>1030</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1010</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1008</v>
+        <v>1027</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1012</v>
+        <v>1031</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1010</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1008</v>
+        <v>1027</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1013</v>
+        <v>1032</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>1010</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1014</v>
+        <v>1033</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>1015</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1014</v>
+        <v>1033</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1011</v>
+        <v>1030</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>1015</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1014</v>
+        <v>1033</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1012</v>
+        <v>1031</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1015</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1014</v>
+        <v>1033</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1013</v>
+        <v>1032</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>1015</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1016</v>
+        <v>1035</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1017</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1018</v>
+        <v>1037</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1017</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1019</v>
+        <v>1038</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1020</v>
+        <v>1039</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1021</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1023</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1011</v>
+        <v>1030</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1024</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1012</v>
+        <v>1031</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1025</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1013</v>
+        <v>1032</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1026</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1027</v>
+        <v>1046</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1028</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1029</v>
+        <v>1048</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1030</v>
+        <v>1049</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1017</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -27107,7 +27470,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1031</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27120,257 +27483,257 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1032</v>
+        <v>1051</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1033</v>
+        <v>1052</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1007</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1034</v>
+        <v>1053</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1035</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1036</v>
+        <v>1055</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1037</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1038</v>
+        <v>1057</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1039</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1040</v>
+        <v>1059</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>1041</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1042</v>
+        <v>1061</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>1043</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1044</v>
+        <v>1063</v>
       </c>
       <c r="B10" s="2" t="n">
         <f aca="false">B8</f>
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>1045</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1046</v>
+        <v>1065</v>
       </c>
       <c r="B11" s="2" t="n">
         <f aca="false">B9/B5</f>
         <v>15</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1047</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1048</v>
+        <v>1067</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>300</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>1049</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1050</v>
+        <v>1069</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>300</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1051</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1052</v>
+        <v>1071</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1053</v>
+        <v>1072</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1054</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1055</v>
+        <v>1074</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1056</v>
+        <v>1075</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1057</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1058</v>
+        <v>1077</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1059</v>
+        <v>1078</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1060</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1061</v>
+        <v>1080</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>561</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1062</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1063</v>
+        <v>1082</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>522</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1064</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1065</v>
+        <v>1084</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>467</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1066</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1067</v>
+        <v>1086</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>359</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1068</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1069</v>
+        <v>1088</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>577</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1070</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1071</v>
+        <v>1090</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>487</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1072</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1073</v>
+        <v>1092</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>327</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>1074</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1075</v>
+        <v>1094</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>326</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>1076</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1077</v>
+        <v>1096</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>287</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>1078</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1079</v>
+        <v>1098</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>629</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>1080</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -27465,50 +27828,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1081</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1082</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>1083</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>1084</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>1085</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1086</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>1087</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>1088</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
-        <v>1089</v>
+        <v>1108</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1090</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27516,7 +27879,7 @@
         <v>587</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1091</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27524,7 +27887,7 @@
         <v>588</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1092</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27532,7 +27895,7 @@
         <v>589</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1093</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27540,7 +27903,7 @@
         <v>590</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1094</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27548,7 +27911,7 @@
         <v>591</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1095</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27556,7 +27919,7 @@
         <v>592</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1096</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27564,7 +27927,7 @@
         <v>593</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1097</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27572,45 +27935,45 @@
         <v>594</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1098</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>1099</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>1100</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1101</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>1102</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>1103</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>1088</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="s">
-        <v>1104</v>
+        <v>1123</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1105</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27618,7 +27981,7 @@
         <v>590</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1106</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27626,7 +27989,7 @@
         <v>639</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>1107</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27634,7 +27997,7 @@
         <v>640</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1108</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27642,7 +28005,7 @@
         <v>641</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1109</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27650,7 +28013,7 @@
         <v>642</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1110</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27658,109 +28021,109 @@
         <v>643</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1111</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1112</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>1113</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>1088</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="2" t="s">
-        <v>1114</v>
+        <v>1133</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>1115</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
-        <v>981</v>
+        <v>1000</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>1116</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="2" t="s">
-        <v>982</v>
+        <v>1001</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1117</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="2" t="s">
-        <v>983</v>
+        <v>1002</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>1118</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="2" t="s">
-        <v>1119</v>
+        <v>1138</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>1120</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>1121</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>1122</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>1123</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>1124</v>
+        <v>1143</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1125</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>1004</v>
+        <v>1023</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1126</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>1005</v>
+        <v>1024</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1127</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>1006</v>
+        <v>1025</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1128</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27768,42 +28131,42 @@
         <v>594</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1129</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>1130</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>1131</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>1132</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>1133</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>1134</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>1135</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>1136</v>
+        <v>1155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>